<commit_message>
Added test for complex invalid URL, improved StaticPagePlugin (images and pdf still don't work), added some test material
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -41,28 +41,7 @@
     <t>Anmerkung</t>
   </si>
   <si>
-    <t>Arthur</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Meeting</t>
-  </si>
-  <si>
     <t>Development</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Recherche</t>
-  </si>
-  <si>
-    <t>Deployment</t>
   </si>
   <si>
     <t>Wichtig! Evtl muss der Datenbereich angepasst werden</t>
@@ -101,7 +80,13 @@
     <t>Pluginsystem überarbeitet</t>
   </si>
   <si>
-    <t>Pluginsystem fertig, Statische Seiten Plugin fertig</t>
+    <t>PluginManager done, lädt plugins dyamisch</t>
+  </si>
+  <si>
+    <t>StaticPage immernoch nicht ganz (bilder/pdf gehen nicht), Test für komplexe invalide URL</t>
+  </si>
+  <si>
+    <t>Pluginsystem fertig, Statische Seiten Plugin fast fertig</t>
   </si>
 </sst>
 </file>
@@ -159,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -171,39 +156,6 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="8"/>
@@ -228,37 +180,6 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="8"/>
@@ -287,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -304,15 +225,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -322,50 +234,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" pivotButton="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,9 +341,6 @@
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -483,7 +365,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deployment</c:v>
+                  <c:v>Grand Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -511,9 +393,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -537,9 +416,6 @@
               <c:f>'Zeitliste Pivot'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Development</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -566,9 +442,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -592,9 +465,6 @@
               <c:f>'Zeitliste Pivot'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Management</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -621,9 +491,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -647,9 +514,6 @@
               <c:f>'Zeitliste Pivot'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Meeting</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -676,12 +540,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -705,9 +563,6 @@
               <c:f>'Zeitliste Pivot'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Recherche</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -734,9 +589,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -761,11 +613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45067264"/>
-        <c:axId val="45073536"/>
+        <c:axId val="41739392"/>
+        <c:axId val="41741312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45067264"/>
+        <c:axId val="41739392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,7 +643,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45073536"/>
+        <c:crossAx val="41741312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -799,7 +651,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45073536"/>
+        <c:axId val="41741312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45067264"/>
+        <c:crossAx val="41739392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -894,34 +746,37 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41557.907581597225" refreshedVersion="4" recordCount="148">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41610.707135416669" refreshedVersion="4" recordCount="148">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-11-21T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
-        <s v="Arthur"/>
-        <s v="Sebastian"/>
+      <sharedItems containsBlank="1" count="5">
+        <s v="Alex"/>
+        <s v="Philipp"/>
         <m/>
+        <s v="Sebastian" u="1"/>
+        <s v="Arthur" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Tätigkeit" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
-        <s v="Management"/>
-        <s v="Meeting"/>
+      <sharedItems containsBlank="1" count="8">
+        <s v="Beginn Projekt"/>
         <s v="Development"/>
-        <s v="Testing"/>
-        <s v="Recherche"/>
-        <s v="Deployment"/>
         <m/>
+        <s v="Deployment" u="1"/>
+        <s v="Meeting" u="1"/>
+        <s v="Testing" u="1"/>
+        <s v="Recherche" u="1"/>
+        <s v="Management" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Dauer (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="4"/>
     </cacheField>
     <cacheField name="Anmerkung" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -938,1038 +793,1038 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="148">
   <r>
-    <s v="1.9.2013"/>
+    <d v="2013-10-03T00:00:00"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="1"/>
-    <s v="Am Sonntag arbeiten kann wenig"/>
-  </r>
-  <r>
-    <s v="2.9.2013"/>
+    <n v="2"/>
+    <s v="IDE eingerichtet, Projekt angelegt, Server angefangen"/>
+  </r>
+  <r>
+    <d v="2013-10-03T00:00:00"/>
     <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
     <n v="2"/>
-    <s v="Bei Kaffee und Kuchen"/>
-  </r>
-  <r>
-    <s v="2.9.2013"/>
+    <s v="IDE eingerichtet, Projekt angelegt, Server angefangen"/>
+  </r>
+  <r>
+    <d v="2013-10-03T00:00:00"/>
     <x v="0"/>
     <x v="1"/>
     <n v="2"/>
-    <s v="Bei Kaffee und Kuchen"/>
-  </r>
-  <r>
-    <s v="2.9.2013"/>
+    <s v="Server mit Multithreading fertig"/>
+  </r>
+  <r>
+    <d v="2013-10-08T00:00:00"/>
     <x v="0"/>
-    <x v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Ansatz Pluginsystem"/>
+  </r>
+  <r>
+    <d v="2013-10-09T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.5"/>
+    <s v="Pluginsystem überarbeitet"/>
+  </r>
+  <r>
+    <d v="2013-10-09T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1.5"/>
+    <s v="Pluginsystem überarbeitet"/>
+  </r>
+  <r>
+    <d v="2013-10-10T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2"/>
+    <s v="Pluginsystem fertig, Statische Seiten Plugin fertig"/>
+  </r>
+  <r>
+    <d v="2013-11-20T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
     <n v="4"/>
-    <s v="Damit was weiter geht"/>
-  </r>
-  <r>
-    <s v="2.9.2013"/>
-    <x v="1"/>
-    <x v="3"/>
-    <n v="1"/>
-    <s v="Fast alles funktioniert"/>
-  </r>
-  <r>
-    <s v="3.9.2013"/>
-    <x v="0"/>
-    <x v="4"/>
-    <n v="2"/>
-    <s v="Was neues versuchen"/>
-  </r>
-  <r>
-    <s v="4.9.2013"/>
-    <x v="1"/>
-    <x v="5"/>
-    <n v="2"/>
-    <s v="Am Server zum Laufen bringen"/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="6"/>
+    <s v="PluginManager done, lädt plugins dyamisch"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
     <m/>
     <m/>
   </r>
@@ -1978,26 +1833,29 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Zeitliste Pivot" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="4">
-  <location ref="A1:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A1:B3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField name="Datum" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Ausführende/r" axis="axisCol" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
+      <items count="6">
+        <item h="1" x="0"/>
+        <item m="1" x="4"/>
+        <item h="1" x="1"/>
+        <item m="1" x="3"/>
         <item h="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField name="Tätigkeit" axis="axisRow" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="8">
-        <item x="5"/>
+      <items count="9">
+        <item x="0"/>
+        <item m="1" x="3"/>
+        <item x="1"/>
+        <item m="1" x="7"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
         <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2007,25 +1865,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
+  <rowItems count="1">
     <i t="grand">
       <x/>
     </i>
@@ -2033,13 +1873,7 @@
   <colFields count="1">
     <field x="1"/>
   </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <colItems count="1">
     <i t="grand">
       <x/>
     </i>
@@ -2341,7 +2175,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2351,13 +2185,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
@@ -2367,13 +2201,13 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
@@ -2400,137 +2234,157 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="A6" s="10">
         <v>41550</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
+      <c r="A7" s="10">
         <v>41550</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
+      <c r="A8" s="10">
         <v>41550</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26">
+      <c r="A9" s="10">
         <v>41555</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26">
+      <c r="A10" s="10">
         <v>41556</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3">
         <v>1.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26">
+      <c r="A11" s="10">
         <v>41556</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3">
         <v>1.5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26">
+      <c r="A12" s="10">
         <v>41557</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="10">
+        <v>41598</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="10">
+        <v>41610</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
@@ -3544,7 +3398,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -3554,119 +3408,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>19</v>
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16">
-        <v>2</v>
-      </c>
-      <c r="D3" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="19">
-        <v>4</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="19">
-        <v>1</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="19">
-        <v>2</v>
-      </c>
-      <c r="C6" s="20">
-        <v>2</v>
-      </c>
-      <c r="D6" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="19">
-        <v>2</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20">
-        <v>1</v>
-      </c>
-      <c r="D8" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="23">
-        <v>9</v>
-      </c>
-      <c r="C9" s="24">
-        <v>5</v>
-      </c>
-      <c r="D9" s="25">
-        <v>14</v>
-      </c>
+      <c r="B3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
StaticPage Plugin done; Started on Navi
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Pluginsystem fertig, Statische Seiten Plugin fast fertig</t>
+  </si>
+  <si>
+    <t>Start Temerature Plugin</t>
+  </si>
+  <si>
+    <t>Temperature Plugin - DB handler klasse "done"</t>
+  </si>
+  <si>
+    <t>StaticPage done, angefangen mit Navi</t>
   </si>
 </sst>
 </file>
@@ -287,11 +296,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-GB"/>
               <a:t>Auswertung</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -613,11 +624,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41739392"/>
-        <c:axId val="41741312"/>
+        <c:axId val="105636992"/>
+        <c:axId val="105638912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41739392"/>
+        <c:axId val="105636992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,17 +644,19 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-GB"/>
                   <a:t>Ausführende/r</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41741312"/>
+        <c:crossAx val="105638912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -651,7 +664,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41741312"/>
+        <c:axId val="105638912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,11 +681,13 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-GB"/>
                   <a:t>Stunden</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -694,13 +709,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41739392"/>
+        <c:crossAx val="105636992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -746,13 +762,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41610.707135416669" refreshedVersion="4" recordCount="148">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41611.643132175923" refreshedVersion="4" recordCount="148">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-11-21T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-12-03T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -839,7 +855,7 @@
     <x v="0"/>
     <x v="1"/>
     <n v="2"/>
-    <s v="Pluginsystem fertig, Statische Seiten Plugin fertig"/>
+    <s v="Pluginsystem fertig, Statische Seiten Plugin fast fertig"/>
   </r>
   <r>
     <d v="2013-11-20T00:00:00"/>
@@ -849,11 +865,11 @@
     <s v="PluginManager done, lädt plugins dyamisch"/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="2"/>
-    <m/>
-    <m/>
+    <d v="2013-12-02T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4"/>
+    <s v="StaticPage immernoch nicht ganz (bilder/pdf gehen nicht), Test für komplexe invalide URL"/>
   </r>
   <r>
     <m/>
@@ -2175,12 +2191,13 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="3"/>
     <col min="5" max="5" width="85" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2371,1020 +2388,910 @@
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
+        <v>41600</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
         <v>41610</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>41610</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D16" s="3">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="1"/>
-    </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="10">
+        <v>41611</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="3"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="3"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="3"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="3"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="3"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="3"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="3"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="3"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="3"/>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="3"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="3"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="3"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="3"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="3"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="3"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="3"/>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="3"/>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="3"/>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="3"/>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="3"/>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="3"/>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="3"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="3"/>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="3"/>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="3"/>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="3"/>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="3"/>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="3"/>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="3"/>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="3"/>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="3"/>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="3"/>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="3"/>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="3"/>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="3"/>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="3"/>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="3"/>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="3"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="3"/>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="3"/>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="3"/>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="3"/>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="3"/>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="3"/>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="3"/>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="3"/>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="3"/>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="3"/>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="3"/>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="3"/>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="3"/>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="3"/>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="3"/>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="3"/>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="3"/>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="3"/>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="3"/>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="3"/>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="3"/>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="3"/>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="3"/>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="3"/>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="3"/>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="3"/>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="3"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="3"/>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="3"/>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="3"/>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="3"/>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="3"/>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="3"/>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="3"/>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="3"/>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="3"/>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="3"/>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="3"/>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="3"/>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="3"/>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
-      <c r="D101" s="3"/>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
-      <c r="D102" s="3"/>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
-      <c r="D103" s="3"/>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
-      <c r="D104" s="3"/>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
-      <c r="D105" s="3"/>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
-      <c r="D106" s="3"/>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
-      <c r="D107" s="3"/>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
-      <c r="D108" s="3"/>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
-      <c r="D109" s="3"/>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
-      <c r="D110" s="3"/>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
-      <c r="D111" s="3"/>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-      <c r="D112" s="3"/>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
-      <c r="D113" s="3"/>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
-      <c r="D114" s="3"/>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
-      <c r="D115" s="3"/>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
-      <c r="D116" s="3"/>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
-      <c r="D117" s="3"/>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
-      <c r="D118" s="3"/>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="3"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
-      <c r="D119" s="3"/>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
-      <c r="D120" s="3"/>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
-      <c r="D121" s="3"/>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
-      <c r="D122" s="3"/>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
-      <c r="D123" s="3"/>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
-      <c r="D124" s="3"/>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="3"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
-      <c r="D125" s="3"/>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="3"/>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
-      <c r="D127" s="3"/>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
-      <c r="D128" s="3"/>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="3"/>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="3"/>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
-      <c r="D131" s="3"/>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
-      <c r="D132" s="3"/>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
-      <c r="D133" s="3"/>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
-      <c r="D134" s="3"/>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
-      <c r="D135" s="3"/>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
-      <c r="D136" s="3"/>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
-      <c r="D137" s="3"/>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
-      <c r="D138" s="3"/>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="3"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
-      <c r="D139" s="3"/>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="3"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
-      <c r="D140" s="3"/>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="3"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="3"/>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="3"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
-      <c r="D142" s="3"/>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="3"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
-      <c r="D143" s="3"/>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="3"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
-      <c r="D144" s="3"/>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="3"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
-      <c r="D145" s="3"/>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="3"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
-      <c r="D146" s="3"/>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="3"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
-      <c r="D147" s="3"/>
       <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="3"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
-      <c r="D148" s="3"/>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="3"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
-      <c r="D149" s="3"/>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
-      <c r="D150" s="3"/>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
-      <c r="D151" s="3"/>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
-      <c r="D152" s="3"/>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
-      <c r="D153" s="3"/>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
-      <c r="D154" s="3"/>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
-      <c r="D155" s="3"/>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
-      <c r="D156" s="3"/>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
-      <c r="D157" s="3"/>
       <c r="E157" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the PluginManger to be Global, Added method to IPlugin, Progress on NaviPlugin
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>StaticPage done, angefangen mit Navi</t>
+  </si>
+  <si>
+    <t>PluginManager jetzt "global", Fortschritt bei Navi</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -624,11 +626,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="105636992"/>
-        <c:axId val="105638912"/>
+        <c:axId val="99157120"/>
+        <c:axId val="99159040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105636992"/>
+        <c:axId val="99157120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,13 +652,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105638912"/>
+        <c:crossAx val="99159040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -664,7 +665,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105638912"/>
+        <c:axId val="99159040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,7 +688,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -709,14 +709,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105636992"/>
+        <c:crossAx val="99157120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -762,13 +761,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41611.643132175923" refreshedVersion="4" recordCount="148">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41620.792229629631" refreshedVersion="4" recordCount="148">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-12-03T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-12-04T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -792,7 +791,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Dauer (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="Anmerkung" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -865,6 +864,20 @@
     <s v="PluginManager done, lädt plugins dyamisch"/>
   </r>
   <r>
+    <d v="2013-11-22T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="5"/>
+    <s v="Start Temerature Plugin"/>
+  </r>
+  <r>
+    <d v="2013-12-02T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+    <s v="Temperature Plugin - DB handler klasse &quot;done&quot;"/>
+  </r>
+  <r>
     <d v="2013-12-02T00:00:00"/>
     <x v="0"/>
     <x v="1"/>
@@ -872,25 +885,11 @@
     <s v="StaticPage immernoch nicht ganz (bilder/pdf gehen nicht), Test für komplexe invalide URL"/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="2"/>
-    <x v="2"/>
-    <m/>
-    <m/>
+    <d v="2013-12-03T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2"/>
+    <s v="StaticPage done, angefangen mit Navi"/>
   </r>
   <r>
     <m/>
@@ -2191,7 +2190,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2455,10 +2454,21 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="10">
+        <v>41620</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>

</xml_diff>

<commit_message>
Navi done, Custom done, some changes
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Navi quasi fertig, paar Encoding Probleme</t>
+  </si>
+  <si>
+    <t>Navi done, Custom done.</t>
   </si>
 </sst>
 </file>
@@ -629,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41682816"/>
-        <c:axId val="41705472"/>
+        <c:axId val="43902080"/>
+        <c:axId val="43904000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41682816"/>
+        <c:axId val="43902080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +663,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41705472"/>
+        <c:crossAx val="43904000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +671,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41705472"/>
+        <c:axId val="43904000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +715,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41682816"/>
+        <c:crossAx val="43902080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -764,13 +767,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41625.72494039352" refreshedVersion="4" recordCount="148">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex" refreshedDate="41641.806871643515" refreshedVersion="4" recordCount="148">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-12-13T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-10-03T00:00:00" maxDate="2013-12-17T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -902,11 +905,11 @@
     <s v="PluginManager jetzt &quot;global&quot;, Fortschritt bei Navi"/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="2"/>
-    <m/>
-    <m/>
+    <d v="2013-12-16T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4"/>
+    <s v="Navi quasi fertig, paar Encoding Probleme"/>
   </r>
   <r>
     <m/>
@@ -2193,7 +2196,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2491,10 +2494,21 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="10">
+        <v>41641</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>

</xml_diff>